<commit_message>
templateDefinition.id => templateDefinition.refid. id for templates added.
</commit_message>
<xml_diff>
--- a/examples/templates/EmploymentContractTemplate.xlsx
+++ b/examples/templates/EmploymentContractTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Java/merlin/examples/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C840D0-9C6E-EF4F-862D-F22BB07F0025}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D95CBF-0A05-2E42-A389-5B856A3BFA6A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6220" yWindow="460" windowWidth="27380" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,9 +183,6 @@
     <t>Date of contract.</t>
   </si>
   <si>
-    <t>Employment contract template</t>
-  </si>
-  <si>
     <t>EmploymentContract-${Employee}</t>
   </si>
   <si>
@@ -205,6 +202,9 @@
   </si>
   <si>
     <t>Find a unique name shortly describing the functionality of this template, e. g. 'Employee contract'. You may refer this definition Excel file by this id.</t>
+  </si>
+  <si>
+    <t>Employment contract definition</t>
   </si>
 </sst>
 </file>
@@ -1000,10 +1000,10 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1014,29 +1014,29 @@
         <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>